<commit_message>
updated open encounters exclusion department file
</commit_message>
<xml_diff>
--- a/open_encounters_exclusion_dept.xlsx
+++ b/open_encounters_exclusion_dept.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kweons01\Desktop\Strategic Initiatives - So Youn\Github\server-upload-updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kweons01\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF33A193-037E-4C91-AE76-79E51ACE9A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="5340" yWindow="1770" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>DEPARTMENT</t>
   </si>
@@ -108,12 +109,18 @@
   </si>
   <si>
     <t>1111 AMST AVE GERI HOME CERTS</t>
+  </si>
+  <si>
+    <t>158 W 124TH ST IAM DENTAL</t>
+  </si>
+  <si>
+    <t>X_440 W 114TH IAM DENTAL_DEACTIVATED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -450,11 +457,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,6 +735,39 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3">
+        <v>8274005</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3">
+        <v>8808068</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="3">
+        <v>43006057</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>